<commit_message>
Added basic functional form/radio button for occupied and empty
</commit_message>
<xml_diff>
--- a/excelsheetsForDatabase/fci_room.xlsx
+++ b/excelsheetsForDatabase/fci_room.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nattb\Coding projects\fcimap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nattb\Coding projects\fcimap\excelsheetsForDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049A998D-7655-4B8C-BC56-755EC02B6A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A36353-3444-400F-B219-130B6B3643E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2606" yWindow="2606" windowWidth="18514" windowHeight="10123" xr2:uid="{B2E91071-72F7-4E7A-9607-581E0EBB8680}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14092" xr2:uid="{B2E91071-72F7-4E7A-9607-581E0EBB8680}"/>
   </bookViews>
   <sheets>
     <sheet name="fci_room" sheetId="1" r:id="rId1"/>
@@ -896,15 +896,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF09183-23BC-4ED5-B180-29EA5348FFD3}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F1" sqref="F1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -921,13 +921,16 @@
       <c r="E1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B40" si="0">"CQ"&amp;C2&amp;"R"&amp;D2*1000+E2</f>
+        <f t="shared" ref="B2:B21" si="0">"CQ"&amp;C2&amp;"R"&amp;D2*1000+E2</f>
         <v>CQAR1002</v>
       </c>
       <c r="C2" t="s">
@@ -939,8 +942,11 @@
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -957,8 +963,11 @@
       <c r="E3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -975,8 +984,11 @@
       <c r="E4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -993,8 +1005,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1011,8 +1026,11 @@
       <c r="E6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1029,8 +1047,11 @@
       <c r="E7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1047,8 +1068,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1065,8 +1089,11 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1083,8 +1110,11 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1101,8 +1131,11 @@
       <c r="E11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1119,8 +1152,11 @@
       <c r="E12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1137,8 +1173,11 @@
       <c r="E13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1155,8 +1194,11 @@
       <c r="E14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1173,8 +1215,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1191,8 +1236,11 @@
       <c r="E16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1209,8 +1257,11 @@
       <c r="E17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1227,8 +1278,11 @@
       <c r="E18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1245,8 +1299,11 @@
       <c r="E19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1263,8 +1320,11 @@
       <c r="E20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1280,6 +1340,9 @@
       </c>
       <c r="E21">
         <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>